<commit_message>
Add instructions to Pipeline Analysis Template
</commit_message>
<xml_diff>
--- a/testfiles/PipelineAnalysisTemplate.xlsx
+++ b/testfiles/PipelineAnalysisTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ELC3338\Spring2018\potter\ARM-Lab\testfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\potterst\Documents\CompOrg\Fall_2018\Day23\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="49">
   <si>
     <t>Fetch</t>
   </si>
@@ -68,6 +68,9 @@
     <t>iE</t>
   </si>
   <si>
+    <t>iM</t>
+  </si>
+  <si>
     <t>iW</t>
   </si>
   <si>
@@ -140,7 +143,34 @@
     <t>sign_extended_output_ie</t>
   </si>
   <si>
-    <t>All</t>
+    <t>Indicates examples that I've already completed for you</t>
+  </si>
+  <si>
+    <t>Indicates signals that go both from left to right and right to left.  For these signals, the Src and Dst columns can be a bit ambiguous</t>
+  </si>
+  <si>
+    <t>Indicates signals that go from right to left and are not forwarded and buffered by the next stage.  pc_src is done for you as an example</t>
+  </si>
+  <si>
+    <t>Instructions:</t>
+  </si>
+  <si>
+    <t>1. Add all of the signals in your datapath to this chart (except for clks and reset).  The signals that I've listed are not necessarily a complete list</t>
+  </si>
+  <si>
+    <t>2. Start by putting the signals in the output column of stage where the signal is generated.</t>
+  </si>
+  <si>
+    <t>3. Determine the final destination of the signal and list this in the Dst column.</t>
+  </si>
+  <si>
+    <t>4. Add that signal as an input to the stage that you listed in the Dst column, listing the Src as the original stage that produced the output signal</t>
+  </si>
+  <si>
+    <t>5. Fill in the intermediate signals that need to be forwarded for the signal to reach its destination.</t>
+  </si>
+  <si>
+    <t>6. You must use the naming convention shown in the examples.  The convention includes the output signal having a suffix that indicates which stage produced the signal</t>
   </si>
 </sst>
 </file>
@@ -182,7 +212,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,6 +231,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -417,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -458,9 +500,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -741,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T29"/>
+  <dimension ref="A1:T41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,61 +852,61 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="T2" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -870,20 +914,20 @@
         <v>9</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="30"/>
+        <v>14</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="19"/>
       <c r="O3" s="19" t="s">
         <v>9</v>
       </c>
@@ -902,20 +946,16 @@
       <c r="B4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>11</v>
-      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="13"/>
       <c r="M4" s="6"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -929,63 +969,65 @@
       <c r="A5" s="6"/>
       <c r="B5" s="1"/>
       <c r="C5" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="17"/>
+        <v>34</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>13</v>
+      </c>
       <c r="I5" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="L5" s="17"/>
+        <v>35</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="M5" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N5" s="16" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="R5" s="16" t="s">
-        <v>11</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="P5" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="11"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="C6" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="E6" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="16" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="1"/>
@@ -1008,11 +1050,11 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>14</v>
+      <c r="E7" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>15</v>
       </c>
       <c r="G7" s="21"/>
       <c r="H7" s="22"/>
@@ -1034,11 +1076,11 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>14</v>
+      <c r="E8" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="34" t="s">
+        <v>15</v>
       </c>
       <c r="G8" s="21"/>
       <c r="H8" s="22"/>
@@ -1060,11 +1102,11 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>14</v>
+      <c r="E9" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="34" t="s">
+        <v>15</v>
       </c>
       <c r="G9" s="21"/>
       <c r="H9" s="22"/>
@@ -1107,7 +1149,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="6"/>
@@ -1131,7 +1173,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="1"/>
       <c r="G12" s="21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="23"/>
@@ -1155,7 +1197,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="1"/>
       <c r="G13" s="21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H13" s="22"/>
       <c r="I13" s="23"/>
@@ -1179,7 +1221,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="1"/>
       <c r="G14" s="21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H14" s="22"/>
       <c r="I14" s="23"/>
@@ -1203,29 +1245,37 @@
       <c r="E15" s="6"/>
       <c r="F15" s="1"/>
       <c r="G15" s="16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I15" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="L15" s="22"/>
-      <c r="M15" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="N15" s="21"/>
-      <c r="O15" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="K15" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="P15" s="22"/>
+      <c r="L15" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M15" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N15" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="O15" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="P15" s="17" t="s">
+        <v>15</v>
+      </c>
       <c r="Q15" s="16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R15" s="16" t="s">
         <v>12</v>
@@ -1241,7 +1291,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="6"/>
@@ -1265,7 +1315,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="1"/>
       <c r="G17" s="21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H17" s="22"/>
       <c r="I17" s="23"/>
@@ -1289,7 +1339,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="1"/>
       <c r="G18" s="21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H18" s="22"/>
       <c r="I18" s="23"/>
@@ -1313,7 +1363,7 @@
       <c r="E19" s="6"/>
       <c r="F19" s="1"/>
       <c r="G19" s="21" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H19" s="22"/>
       <c r="I19" s="21"/>
@@ -1337,7 +1387,7 @@
       <c r="E20" s="6"/>
       <c r="F20" s="1"/>
       <c r="G20" s="21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H20" s="22"/>
       <c r="I20" s="21"/>
@@ -1361,7 +1411,7 @@
       <c r="E21" s="6"/>
       <c r="F21" s="1"/>
       <c r="G21" s="21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H21" s="22"/>
       <c r="I21" s="23"/>
@@ -1549,6 +1599,59 @@
       <c r="S29" s="1"/>
       <c r="T29" s="11"/>
     </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="30"/>
+      <c r="C31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" s="31"/>
+      <c r="C32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="32"/>
+      <c r="C33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:D1"/>

</xml_diff>